<commit_message>
update backend to work with more stock tickers
</commit_message>
<xml_diff>
--- a/backend/IR_website_links.xlsx
+++ b/backend/IR_website_links.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c0e4e62c6ea45fc4/General/Projects/Earning release warnings/backend/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\stockpulse\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{1678C1A8-BA36-4DA7-9513-CE5705F5EACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15C52312-29EC-4205-9AB4-FD55302CD15E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4446FC5-42AC-49F9-AAFC-F60A35783643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE7E914D-695C-4B9F-90FE-B40BE7A7AD48}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE7E914D-695C-4B9F-90FE-B40BE7A7AD48}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Ticker</t>
   </si>
@@ -59,12 +59,6 @@
     <t>TEAM</t>
   </si>
   <si>
-    <t>NFLX</t>
-  </si>
-  <si>
-    <t>MSFT</t>
-  </si>
-  <si>
     <t>https://investor.fb.com/home/default.aspx</t>
   </si>
   <si>
@@ -77,19 +71,43 @@
     <t>https://s28.q4cdn.com/541786762/files/doc_financials/2024/q2/TEAM-Q2-2024-Earnings-Release.pdf</t>
   </si>
   <si>
-    <t>https://ir.netflix.net/ir-overview/profile/default.aspx</t>
-  </si>
-  <si>
-    <t>https://s22.q4cdn.com/959853165/files/doc_financials/2023/q4/NEW-FINAL-Q4-23-Shareholder-Letter.pdf</t>
-  </si>
-  <si>
-    <t>https://www.microsoft.com/en-us/investor</t>
-  </si>
-  <si>
-    <t>https://view.officeapps.live.com/op/view.aspx?src=https://c.s-microsoft.com/en-us/CMSFiles/PressReleaseFY24Q2.docx?version=6dc37440-3219-dd39-05a0-c3218a72482b</t>
-  </si>
-  <si>
     <t>Latest_press_release_link</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>https://s201.q4cdn.com/336605034/files/doc_earnings/2023/q4/earnings-result/WBD-4Q23-Earnings-Release.pdf</t>
+  </si>
+  <si>
+    <t>WBD</t>
+  </si>
+  <si>
+    <t>Warner Bros. Discovery, Inc.</t>
+  </si>
+  <si>
+    <t>https://ir.corporate.discovery.com/investor-relations/default.aspx</t>
+  </si>
+  <si>
+    <t>Moderna, Inc.</t>
+  </si>
+  <si>
+    <t>MRNA</t>
+  </si>
+  <si>
+    <t>https://investors.modernatx.com/overview/default.aspx</t>
+  </si>
+  <si>
+    <t>https://s29.q4cdn.com/435878511/files/doc_earnings/2023/q4/earnings-result/Q4-23-PR_Final.pdf</t>
+  </si>
+  <si>
+    <t>Atlassian Corporation</t>
+  </si>
+  <si>
+    <t>Meta Platforms, Inc.</t>
+  </si>
+  <si>
+    <t>Alphabet Inc.</t>
   </si>
 </sst>
 </file>
@@ -134,9 +152,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -472,7 +493,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA113124-681D-4A1B-94A2-B1B5EAFDA1C2}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
@@ -480,88 +501,106 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="47.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="91.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="3" max="3" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="104.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>17</v>
+      <c r="D1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
+      <c r="B3" t="s">
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{16BB405E-D988-41C0-9031-D20966EBD4A5}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{D1363808-8DF2-4865-9798-93CA02F5CFF0}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{16AA8084-B8AB-489A-AE10-0E5EBDD00552}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{7FE7701F-5DEA-4AF3-A22B-699B2AB2DD6F}"/>
-    <hyperlink ref="B4" r:id="rId5" xr:uid="{59CA3982-270A-4B47-8FF7-869B1E881763}"/>
-    <hyperlink ref="C4" r:id="rId6" xr:uid="{99631F2F-4054-43E3-8447-B8C1CC229FF1}"/>
-    <hyperlink ref="B5" r:id="rId7" xr:uid="{740C0386-C0B0-4B9A-AC94-629A3A567134}"/>
-    <hyperlink ref="C5" r:id="rId8" xr:uid="{04E2437E-9D22-4247-A88B-EBABF97CDCD6}"/>
-    <hyperlink ref="B6" r:id="rId9" xr:uid="{2CD3B584-EF14-4682-AD45-B9DF8F822232}"/>
-    <hyperlink ref="C6" r:id="rId10" xr:uid="{3CDE1683-23E0-4CD7-896B-89CDC89E578D}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{16BB405E-D988-41C0-9031-D20966EBD4A5}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{D1363808-8DF2-4865-9798-93CA02F5CFF0}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{16AA8084-B8AB-489A-AE10-0E5EBDD00552}"/>
+    <hyperlink ref="D3" r:id="rId4" xr:uid="{7FE7701F-5DEA-4AF3-A22B-699B2AB2DD6F}"/>
+    <hyperlink ref="C4" r:id="rId5" xr:uid="{59CA3982-270A-4B47-8FF7-869B1E881763}"/>
+    <hyperlink ref="D4" r:id="rId6" xr:uid="{99631F2F-4054-43E3-8447-B8C1CC229FF1}"/>
+    <hyperlink ref="C5" r:id="rId7" xr:uid="{9810E13B-10FF-485E-9581-97C0E26C6176}"/>
+    <hyperlink ref="C6" r:id="rId8" xr:uid="{A4A97989-5C2B-4E01-80D3-FE1F1A54F3A6}"/>
+    <hyperlink ref="D6" r:id="rId9" xr:uid="{02EF94B1-9A32-4E1B-952D-19236DF21D05}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>